<commit_message>
updated the readme, and worked with bash script to replicate software. Got asynchronous input working
</commit_message>
<xml_diff>
--- a/resources/display-o-tron PINOUT schematic.xlsx
+++ b/resources/display-o-tron PINOUT schematic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidverweij/gitrepos/iotcanvas/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{896401D5-04AE-5E41-99AC-BCF671FF23E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F892EA7A-7F2D-8D49-8B93-A76311545CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29120" yWindow="-180" windowWidth="20680" windowHeight="22700" xr2:uid="{080D51BC-337E-D64D-8596-E43468DA4F0F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>NC</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t xml:space="preserve">3.3V + </t>
+  </si>
+  <si>
+    <t>CAPACITOR A (1uF) +</t>
+  </si>
+  <si>
+    <t>CAPACITOR A (1uF) -  &amp; 3.3V +</t>
+  </si>
+  <si>
+    <t>CAPACITOR B (1uF) +</t>
+  </si>
+  <si>
+    <t>CAPACITOR B (1uF) -</t>
+  </si>
+  <si>
+    <t>SI   (also called MOSI)</t>
+  </si>
+  <si>
+    <t>CSB (also called CE)</t>
+  </si>
+  <si>
+    <t>CLK (also called SCLK)</t>
+  </si>
+  <si>
+    <t>See also: https://github.com/Gadgetoid/DogLCD</t>
   </si>
 </sst>
 </file>
@@ -552,7 +576,7 @@
   <dimension ref="J2:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC23" sqref="AC23"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,7 +595,9 @@
       </c>
     </row>
     <row r="3" spans="10:27" x14ac:dyDescent="0.2">
-      <c r="N3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="10:27" x14ac:dyDescent="0.2">
       <c r="N4" s="4" t="s">
@@ -606,6 +632,9 @@
       <c r="R8" t="s">
         <v>25</v>
       </c>
+      <c r="AA8" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="10:27" x14ac:dyDescent="0.2">
       <c r="J9" s="1" t="s">
@@ -626,6 +655,9 @@
       <c r="R9" t="s">
         <v>25</v>
       </c>
+      <c r="AA9" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L10" s="1">
@@ -657,6 +689,9 @@
       <c r="R11" t="s">
         <v>26</v>
       </c>
+      <c r="AA11" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L12" s="1">
@@ -671,6 +706,9 @@
       <c r="R12" t="s">
         <v>27</v>
       </c>
+      <c r="AA12" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L13" s="1">
@@ -685,6 +723,9 @@
       <c r="R13" t="s">
         <v>28</v>
       </c>
+      <c r="AA13" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L14" s="1">
@@ -699,6 +740,9 @@
       <c r="R14" t="s">
         <v>29</v>
       </c>
+      <c r="AA14" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L15" s="1">
@@ -713,6 +757,9 @@
       <c r="R15" t="s">
         <v>30</v>
       </c>
+      <c r="AA15" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L16" s="1">
@@ -727,6 +774,9 @@
       <c r="R16" t="s">
         <v>31</v>
       </c>
+      <c r="AA16" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L17" s="1">
@@ -741,6 +791,9 @@
       <c r="R17" t="s">
         <v>31</v>
       </c>
+      <c r="AA17" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L18" s="1">
@@ -755,6 +808,9 @@
       <c r="R18" t="s">
         <v>31</v>
       </c>
+      <c r="AA18" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L19" s="1">
@@ -769,6 +825,9 @@
       <c r="R19" t="s">
         <v>31</v>
       </c>
+      <c r="AA19" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L20" s="1">
@@ -783,6 +842,9 @@
       <c r="R20" t="s">
         <v>31</v>
       </c>
+      <c r="AA20" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="21" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L21" s="1">
@@ -797,6 +859,9 @@
       <c r="R21" t="s">
         <v>31</v>
       </c>
+      <c r="AA21" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L22" s="1">
@@ -811,6 +876,9 @@
       <c r="R22" t="s">
         <v>32</v>
       </c>
+      <c r="AA22" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L23" s="1">
@@ -825,6 +893,9 @@
       <c r="R23" t="s">
         <v>33</v>
       </c>
+      <c r="AA23" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L24" s="1">
@@ -839,6 +910,9 @@
       <c r="R24" t="s">
         <v>34</v>
       </c>
+      <c r="AA24" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="10:27" x14ac:dyDescent="0.2">
       <c r="L25" s="1">
@@ -854,7 +928,7 @@
         <v>36</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="10:27" x14ac:dyDescent="0.2">
@@ -875,6 +949,9 @@
       </c>
       <c r="R26" t="s">
         <v>37</v>
+      </c>
+      <c r="AA26" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="10:27" x14ac:dyDescent="0.2">

</xml_diff>